<commit_message>
correct other search directories
</commit_message>
<xml_diff>
--- a/testdata/demo/test.xlsx
+++ b/testdata/demo/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/private/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmichaels/repos/cgap/submitr/testdata/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C593E2D5-66C5-724B-95E3-F9BC9EF33A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F2ECF3-CCD0-EA4C-8BF9-6444E5C4A47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FileFormat" sheetId="1" r:id="rId1"/>
@@ -182,10 +182,10 @@
     <t>asdfadf</t>
   </si>
   <si>
-    <t>smaht:reference_file-fastq100</t>
-  </si>
-  <si>
-    <t>smaht:reference_file-fastq200|smaht:reference_file-fastq_alt-200</t>
+    <t>smaht:reference_file-B</t>
+  </si>
+  <si>
+    <t>smaht:reference_file-A</t>
   </si>
 </sst>
 </file>
@@ -519,8 +519,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -604,7 +604,7 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="A1153" sqref="A8:XFD1153"/>
     </sheetView>
   </sheetViews>

</xml_diff>